<commit_message>
Update factor panel 1) added skimr histograms 2) remove tabs on factor panel 3) added more factors to sample data file
</commit_message>
<xml_diff>
--- a/data/otut_f4.xlsx
+++ b/data/otut_f4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="-2740" windowWidth="26400" windowHeight="16580" activeTab="1"/>
+    <workbookView xWindow="35480" yWindow="-2360" windowWidth="26400" windowHeight="16580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="otut" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="41">
   <si>
     <t>Synergistetes</t>
   </si>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I36"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AC36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3917,15 +3917,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F1" sqref="F1:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -3935,8 +3935,23 @@
       <c r="C1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3946,8 +3961,23 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0.13184584178499001</v>
+      </c>
+      <c r="E2">
+        <v>0.49565343378730797</v>
+      </c>
+      <c r="F2">
+        <v>6.5198493190379604E-3</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>3.5496957403651101E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3957,8 +3987,23 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>9.0329436769394297E-3</v>
+      </c>
+      <c r="E3">
+        <v>0.62539851222104104</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -3968,8 +4013,23 @@
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>4.24E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.57120000000000004</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -3979,8 +4039,23 @@
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>7.22789115646258E-3</v>
+      </c>
+      <c r="E5">
+        <v>0.69345238095238104</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -3990,8 +4065,23 @@
       <c r="C6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>5.6903196554069398E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.48651099523917501</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -4001,8 +4091,23 @@
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>3.3613445378151301E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.74976657329598495</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -4012,8 +4117,23 @@
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>7.6261243644896396E-3</v>
+      </c>
+      <c r="E8">
+        <v>0.288032850997262</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -4023,8 +4143,23 @@
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>3.3193570929419998E-3</v>
+      </c>
+      <c r="E9">
+        <v>0.27742837176799401</v>
+      </c>
+      <c r="F9">
+        <v>5.2410901467505201E-4</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -4034,8 +4169,23 @@
       <c r="C10">
         <v>1.7868404456590299E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>0.14862308177422701</v>
+      </c>
+      <c r="E10">
+        <v>0.40655875551818399</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -4045,8 +4195,23 @@
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>0.207620697120589</v>
+      </c>
+      <c r="E11">
+        <v>0.54275817276466798</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -4056,8 +4221,23 @@
       <c r="C12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>7.00615174299385E-3</v>
+      </c>
+      <c r="E12">
+        <v>0.69890635680109403</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -4067,8 +4247,23 @@
       <c r="C13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>2.0953602736797101E-2</v>
+      </c>
+      <c r="E13">
+        <v>0.88903143040410504</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>4.2762454564892002E-4</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -4078,8 +4273,23 @@
       <c r="C14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>1.1887503624238901E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.661061177152798</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -4089,8 +4299,23 @@
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>9.4665938467139998E-3</v>
+      </c>
+      <c r="E15">
+        <v>0.72437647915528902</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -4100,8 +4325,23 @@
       <c r="C16">
         <v>5.4724553082816504E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>1.34987230937614E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.29587741700109399</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -4111,8 +4351,23 @@
       <c r="C17">
         <v>1.57803376992268E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>7.8586081742149302E-2</v>
+      </c>
+      <c r="E17">
+        <v>0.71106201672715796</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -4122,8 +4377,23 @@
       <c r="C18">
         <v>2.4915908807773802E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>7.37510900710103E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.60545658402890201</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1.2457954403886901E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -4133,8 +4403,23 @@
       <c r="C19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>3.2427695004382098E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.51752848378615202</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -4144,8 +4429,23 @@
       <c r="C20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>1.7686285879965201E-2</v>
+      </c>
+      <c r="E20">
+        <v>0.84169324441867199</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -4155,8 +4455,23 @@
       <c r="C21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>0.12984942426926499</v>
+      </c>
+      <c r="E21">
+        <v>0.54189548272807797</v>
+      </c>
+      <c r="F21">
+        <v>5.3144375553587197E-4</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -4166,8 +4481,23 @@
       <c r="C22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>4.8144064682102201E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.76074972436604205</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -4177,8 +4507,23 @@
       <c r="C23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>1.9434864564762701E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.61271781887660204</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>4.7709923664122098E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -4188,8 +4533,23 @@
       <c r="C24">
         <v>9.9641291351135902E-5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>0.21723253512384999</v>
+      </c>
+      <c r="E24">
+        <v>0.47953107471994699</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -4199,8 +4559,23 @@
       <c r="C25">
         <v>3.06891652043223E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>5.3170276519200303E-2</v>
+      </c>
+      <c r="E25">
+        <v>0.48310675486565502</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -4210,8 +4585,23 @@
       <c r="C26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>9.8401068990169094E-2</v>
+      </c>
+      <c r="E26">
+        <v>0.601454760346813</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>8.8589652728561294E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -4221,8 +4611,23 @@
       <c r="C27">
         <v>3.61769807543288E-4</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>1.54240932474325E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.70046220254323699</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -4232,8 +4637,23 @@
       <c r="C28">
         <v>1.1695863239782799E-4</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>5.39887289693309E-2</v>
+      </c>
+      <c r="E28">
+        <v>0.60827183265084594</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>2.6875940657923001E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -4243,8 +4663,23 @@
       <c r="C29">
         <v>3.4319648682340702E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>0.149784736433139</v>
+      </c>
+      <c r="E29">
+        <v>0.464733677078145</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -4254,8 +4689,23 @@
       <c r="C30">
         <v>1.5421848182952599E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>0.14692987578635699</v>
+      </c>
+      <c r="E30">
+        <v>0.50867965191984099</v>
+      </c>
+      <c r="F30">
+        <v>1.3260534011851001E-4</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1.09155410015009E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -4265,8 +4715,23 @@
       <c r="C31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>7.7177946693426702E-2</v>
+      </c>
+      <c r="E31">
+        <v>0.437157733500807</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -4276,24 +4741,69 @@
       <c r="C32">
         <v>3.9456435669485796E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>2.50126726728544E-2</v>
+      </c>
+      <c r="E32">
+        <v>7.2107116213282002E-2</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>2.2533297133682101E-2</v>
+      </c>
+      <c r="E33">
+        <v>0.17128528559407799</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>1.22870249017038E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>0.10435988525686</v>
+      </c>
+      <c r="E34">
+        <v>0.374721064457542</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -4303,8 +4813,23 @@
       <c r="C35">
         <v>3.2540518267557901E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>0.22553264383537799</v>
+      </c>
+      <c r="E35">
+        <v>0.36397256197609601</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -4313,6 +4838,21 @@
       </c>
       <c r="C36">
         <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0.20793110615237001</v>
+      </c>
+      <c r="E36">
+        <v>0.44234117339602802</v>
+      </c>
+      <c r="F36">
+        <v>7.4306472919418798E-4</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>2.7279130071670998E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>